<commit_message>
Calculating Discharge for new inflow days. Making excel workbook for volumetric inflow days to calculate discharge in L/s per each site
</commit_message>
<xml_diff>
--- a/Inflow/CCR_VolumetricFlow_discharge_data_25aug2020.xlsx
+++ b/Inflow/CCR_VolumetricFlow_discharge_data_25aug2020.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/595e4f0f07ac9838/Desktop/R_Projects/CCR_preliminary/Inflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FF35ED-D009-459E-9174-B2E583B0C5AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{80FF35ED-D009-459E-9174-B2E583B0C5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678589AC-EEBF-4061-ACC3-5D10D7764B65}"/>
   <bookViews>
-    <workbookView xWindow="1596" yWindow="888" windowWidth="12408" windowHeight="10476"/>
+    <workbookView xWindow="35055" yWindow="3960" windowWidth="19530" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCR_VolumetricFlow_discharge_da" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -67,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -902,16 +913,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>